<commit_message>
Progress update and addition of exercise folder
</commit_message>
<xml_diff>
--- a/LPTHW_Progress_Tracker.xlsx
+++ b/LPTHW_Progress_Tracker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ligaya/Dropbox/CODING/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ligaya/Dropbox/CODING/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Table Of Contents</t>
   </si>
@@ -210,9 +210,6 @@
   </si>
   <si>
     <t>Progress</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
   <si>
     <r>
@@ -323,7 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -340,12 +337,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -363,6 +363,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -403,6 +413,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -682,7 +702,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,8 +732,8 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>61</v>
+      <c r="B3" s="10">
+        <v>43109</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -721,14 +741,18 @@
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="10">
+        <v>43109</v>
+      </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="10">
+        <v>43109</v>
+      </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.25">
@@ -912,7 +936,7 @@
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.25">
@@ -1096,7 +1120,7 @@
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.25">
@@ -1122,10 +1146,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B60">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",B3)))</formula>
+    <cfRule type="notContainsBlanks" dxfId="6" priority="3">
+      <formula>LEN(TRIM(B3))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="3" priority="1">
+    <cfRule type="containsBlanks" dxfId="7" priority="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1190,5 +1214,6 @@
     <hyperlink ref="A60" r:id="rId58"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Progress tracker and notes updated
</commit_message>
<xml_diff>
--- a/LPTHW_Progress_Tracker.xlsx
+++ b/LPTHW_Progress_Tracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12080" windowHeight="19620" tabRatio="500"/>
+    <workbookView xWindow="12700" yWindow="460" windowWidth="12080" windowHeight="19620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -488,21 +488,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -782,7 +782,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -875,56 +875,72 @@
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="10">
+        <v>43110</v>
+      </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="10">
+        <v>43110</v>
+      </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="10">
+        <v>43110</v>
+      </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="7"/>
+      <c r="B13" s="10">
+        <v>43110</v>
+      </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="10">
+        <v>43110</v>
+      </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="7"/>
+      <c r="B15" s="10">
+        <v>43110</v>
+      </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="7"/>
+      <c r="B16" s="10">
+        <v>43110</v>
+      </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="7"/>
+      <c r="B17" s="10">
+        <v>43110</v>
+      </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.25">
@@ -1234,10 +1250,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B60">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="3">
       <formula>LEN(TRIM(B3))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="15" priority="1">
+    <cfRule type="containsBlanks" dxfId="14" priority="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>